<commit_message>
Work on submitting Strassen's
</commit_message>
<xml_diff>
--- a/crossovers_experiments.xlsx
+++ b/crossovers_experiments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VICTOR\Harvard_Junior_2019-20\CS 124\CS124_psets\cs124-pa2-cw-vq\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB0BB4B-8EE9-45A1-8FEF-A412C94F6696}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7FD8801-C084-4BD9-9CDF-2BBC3AAEF55F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="3" xr2:uid="{4FFF3968-23DE-45E5-9B4E-6E4BCC278512}"/>
   </bookViews>
@@ -6650,6 +6650,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Crossover</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Points for Even Dimensions</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6904,475 +6934,15 @@
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="8"/>
-          <c:order val="8"/>
+          <c:idx val="13"/>
+          <c:order val="13"/>
           <c:tx>
-            <c:v>40</c:v>
+            <c:v>68</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent3">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3">
-                    <a:lumMod val="60000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Crossover Evens'!$A$91:$A$99</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>256</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>288</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>320</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>352</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>384</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>416</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>448</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>480</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>512</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Crossover Evens'!$D$91:$D$99</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>0.129555</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.17181199999999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.234626</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.31314799999999998</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.41129300000000002</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.50698799999999999</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.65803699999999998</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.74580100000000005</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.87202999999999997</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000008-FEFD-47EF-8966-30805A4459CC}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="9"/>
-          <c:order val="9"/>
-          <c:tx>
-            <c:v>44</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4">
-                    <a:lumMod val="60000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Crossover Evens'!$A$109:$A$117</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>256</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>288</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>320</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>352</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>384</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>416</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>448</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>480</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>512</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Crossover Evens'!$D$109:$D$117</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>0.122033</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.218032</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.24024300000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.32571800000000001</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.42416799999999999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.500112</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.65186500000000003</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.76257200000000003</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.90410199999999996</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000009-FEFD-47EF-8966-30805A4459CC}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="10"/>
-          <c:order val="10"/>
-          <c:tx>
-            <c:v>46</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent5">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent5">
-                    <a:lumMod val="60000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Crossover Evens'!$A$118:$A$126</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>256</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>288</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>320</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>352</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>384</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>416</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>448</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>480</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>512</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Crossover Evens'!$D$118:$D$126</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>0.12679399999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.17943799999999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.22573399999999999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.29196499999999997</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.41719299999999998</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.50188699999999997</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.66224499999999997</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.73905799999999999</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.88100000000000001</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000A-FEFD-47EF-8966-30805A4459CC}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="11"/>
-          <c:order val="11"/>
-          <c:tx>
-            <c:v>50</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent6">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent6">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent6">
-                    <a:lumMod val="60000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Crossover Evens'!$A$136:$A$144</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>256</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>288</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>320</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>352</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>384</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>416</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>448</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>480</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>512</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Crossover Evens'!$D$136:$D$144</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>0.19676199999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.19131999999999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.24840999999999999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.33150000000000002</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.423398</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.53696699999999997</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.69557899999999995</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.78705199999999997</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.93900499999999998</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000B-FEFD-47EF-8966-30805A4459CC}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="12"/>
-          <c:order val="12"/>
-          <c:tx>
-            <c:v>52</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1">
+                <a:schemeClr val="accent2">
                   <a:lumMod val="80000"/>
                   <a:lumOff val="20000"/>
                 </a:schemeClr>
@@ -7386,14 +6956,14 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1">
+                <a:schemeClr val="accent2">
                   <a:lumMod val="80000"/>
                   <a:lumOff val="20000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1">
+                  <a:schemeClr val="accent2">
                     <a:lumMod val="80000"/>
                     <a:lumOff val="20000"/>
                   </a:schemeClr>
@@ -7404,7 +6974,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Crossover Evens'!$A$145:$A$153</c:f>
+              <c:f>'Crossover Evens'!$A$217:$A$225</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -7440,36 +7010,36 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Crossover Evens'!$D$145:$D$153</c:f>
+              <c:f>'Crossover Evens'!$D$217:$D$225</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.19081999999999999</c:v>
+                  <c:v>0.136322</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.187218</c:v>
+                  <c:v>0.18839700000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.243926</c:v>
+                  <c:v>0.26441300000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.317996</c:v>
+                  <c:v>0.30410999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.39557199999999998</c:v>
+                  <c:v>0.41448099999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.54347400000000001</c:v>
+                  <c:v>0.51439599999999996</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.67679199999999995</c:v>
+                  <c:v>0.69649700000000003</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.76576599999999995</c:v>
+                  <c:v>0.763243</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.93206199999999995</c:v>
+                  <c:v>0.97328700000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7477,7 +7047,125 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000D-FEFD-47EF-8966-30805A4459CC}"/>
+              <c16:uniqueId val="{00000000-F031-460F-99F7-114C5AD7A810}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="14"/>
+          <c:order val="14"/>
+          <c:tx>
+            <c:v>16</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="80000"/>
+                    <a:lumOff val="20000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Crossover Evens'!$S$4:$S$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>288</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>352</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>384</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>416</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>448</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>512</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Crossover Evens'!$V$4:$V$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.16816500000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.26289899999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.33520299999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.426126</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.56040599999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.597109</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.78029599999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.89319999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.06864</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7F35-4C3F-8448-286283BDFCB3}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -7649,7 +7337,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Crossover Evens'!$A$19:$A$27</c15:sqref>
@@ -7691,7 +7379,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Crossover Evens'!$D$19:$D$27</c15:sqref>
@@ -7732,7 +7420,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-FEFD-47EF-8966-30805A4459CC}"/>
                   </c:ext>
@@ -7772,7 +7460,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Crossover Evens'!$A$28:$A$36</c15:sqref>
@@ -7814,7 +7502,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Crossover Evens'!$D$28:$D$36</c15:sqref>
@@ -7855,7 +7543,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000003-FEFD-47EF-8966-30805A4459CC}"/>
                   </c:ext>
@@ -7895,7 +7583,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Crossover Evens'!$A$181:$A$189</c15:sqref>
@@ -7937,7 +7625,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Crossover Evens'!$D$181:$D$189</c15:sqref>
@@ -7978,7 +7666,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000005-FEFD-47EF-8966-30805A4459CC}"/>
                   </c:ext>
@@ -8024,7 +7712,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Crossover Evens'!$A$136:$A$144</c15:sqref>
@@ -8066,7 +7754,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Crossover Evens'!$D$136:$D$144</c15:sqref>
@@ -8107,7 +7795,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000006-FEFD-47EF-8966-30805A4459CC}"/>
                   </c:ext>
@@ -8153,7 +7841,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Crossover Evens'!$A$64:$A$72</c15:sqref>
@@ -8195,7 +7883,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Crossover Evens'!$D$64:$D$72</c15:sqref>
@@ -8236,9 +7924,657 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000007-FEFD-47EF-8966-30805A4459CC}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="8"/>
+                <c:order val="8"/>
+                <c:tx>
+                  <c:v>40</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="19050" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent3">
+                        <a:lumMod val="60000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent3">
+                        <a:lumMod val="60000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent3">
+                          <a:lumMod val="60000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Crossover Evens'!$A$91:$A$99</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="9"/>
+                      <c:pt idx="0">
+                        <c:v>256</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>288</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>320</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>352</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>384</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>416</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>448</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>480</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>512</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Crossover Evens'!$D$91:$D$99</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="9"/>
+                      <c:pt idx="0">
+                        <c:v>0.129555</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.17181199999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0.234626</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0.31314799999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0.41129300000000002</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0.50698799999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>0.65803699999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>0.74580100000000005</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>0.87202999999999997</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="0"/>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000008-FEFD-47EF-8966-30805A4459CC}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="9"/>
+                <c:order val="9"/>
+                <c:tx>
+                  <c:v>44</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="19050" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent4">
+                        <a:lumMod val="60000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent4">
+                        <a:lumMod val="60000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent4">
+                          <a:lumMod val="60000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Crossover Evens'!$A$109:$A$117</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="9"/>
+                      <c:pt idx="0">
+                        <c:v>256</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>288</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>320</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>352</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>384</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>416</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>448</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>480</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>512</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Crossover Evens'!$D$109:$D$117</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="9"/>
+                      <c:pt idx="0">
+                        <c:v>0.122033</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.218032</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0.24024300000000001</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0.32571800000000001</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0.42416799999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0.500112</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>0.65186500000000003</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>0.76257200000000003</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>0.90410199999999996</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="0"/>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000009-FEFD-47EF-8966-30805A4459CC}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="10"/>
+                <c:order val="10"/>
+                <c:tx>
+                  <c:v>46</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="19050" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent5">
+                        <a:lumMod val="60000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent5">
+                        <a:lumMod val="60000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent5">
+                          <a:lumMod val="60000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Crossover Evens'!$A$118:$A$126</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="9"/>
+                      <c:pt idx="0">
+                        <c:v>256</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>288</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>320</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>352</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>384</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>416</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>448</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>480</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>512</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Crossover Evens'!$D$118:$D$126</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="9"/>
+                      <c:pt idx="0">
+                        <c:v>0.12679399999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.17943799999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0.22573399999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0.29196499999999997</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0.41719299999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0.50188699999999997</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>0.66224499999999997</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>0.73905799999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>0.88100000000000001</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="0"/>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{0000000A-FEFD-47EF-8966-30805A4459CC}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="11"/>
+                <c:order val="11"/>
+                <c:tx>
+                  <c:v>50</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="19050" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent6">
+                        <a:lumMod val="60000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent6">
+                        <a:lumMod val="60000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent6">
+                          <a:lumMod val="60000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Crossover Evens'!$A$136:$A$144</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="9"/>
+                      <c:pt idx="0">
+                        <c:v>256</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>288</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>320</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>352</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>384</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>416</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>448</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>480</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>512</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Crossover Evens'!$D$136:$D$144</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="9"/>
+                      <c:pt idx="0">
+                        <c:v>0.19676199999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.19131999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0.24840999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0.33150000000000002</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0.423398</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0.53696699999999997</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>0.69557899999999995</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>0.78705199999999997</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>0.93900499999999998</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="0"/>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{0000000B-FEFD-47EF-8966-30805A4459CC}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="12"/>
+                <c:order val="12"/>
+                <c:tx>
+                  <c:v>52</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="19050" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1">
+                        <a:lumMod val="80000"/>
+                        <a:lumOff val="20000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent1">
+                        <a:lumMod val="80000"/>
+                        <a:lumOff val="20000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent1">
+                          <a:lumMod val="80000"/>
+                          <a:lumOff val="20000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Crossover Evens'!$A$145:$A$153</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="9"/>
+                      <c:pt idx="0">
+                        <c:v>256</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>288</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>320</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>352</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>384</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>416</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>448</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>480</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>512</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Crossover Evens'!$D$145:$D$153</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="9"/>
+                      <c:pt idx="0">
+                        <c:v>0.19081999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.187218</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0.243926</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0.317996</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0.39557199999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0.54347400000000001</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>0.67679199999999995</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>0.76576599999999995</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>0.93206199999999995</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="0"/>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{0000000D-FEFD-47EF-8966-30805A4459CC}"/>
                   </c:ext>
                 </c:extLst>
               </c15:ser>
@@ -8267,6 +8603,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Dimension</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> of Matrix</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -8329,6 +8725,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Avg. runtime (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -8378,6 +8829,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -8973,7 +9455,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet5!$A$28:$A$36</c15:sqref>
@@ -9015,7 +9497,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet5!$D$28:$D$36</c15:sqref>
@@ -9056,7 +9538,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000001-4377-4944-89FF-FDBE4FB411D0}"/>
                   </c:ext>
@@ -9096,7 +9578,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet5!$A$172:$A$180</c15:sqref>
@@ -9138,7 +9620,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet5!$D$172:$D$180</c15:sqref>
@@ -9179,7 +9661,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-4377-4944-89FF-FDBE4FB411D0}"/>
                   </c:ext>
@@ -9219,7 +9701,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet5!$A$82:$A$90</c15:sqref>
@@ -9261,7 +9743,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet5!$D$82:$D$90</c15:sqref>
@@ -9302,7 +9784,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000003-4377-4944-89FF-FDBE4FB411D0}"/>
                   </c:ext>
@@ -9348,7 +9830,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet5!$A$136:$A$144</c15:sqref>
@@ -9390,7 +9872,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet5!$D$136:$D$144</c15:sqref>
@@ -9431,7 +9913,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000007-4377-4944-89FF-FDBE4FB411D0}"/>
                   </c:ext>
@@ -9477,7 +9959,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet5!$A$145:$A$153</c15:sqref>
@@ -9519,7 +10001,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet5!$D$145:$D$153</c15:sqref>
@@ -9560,7 +10042,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000008-4377-4944-89FF-FDBE4FB411D0}"/>
                   </c:ext>
@@ -9760,6 +10242,66 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Crossover</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Points for Odd Dimensions</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -9767,15 +10309,15 @@
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
+          <c:idx val="0"/>
+          <c:order val="0"/>
           <c:tx>
-            <c:v>65</c:v>
+            <c:v>37</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent4"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -9786,11 +10328,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent4"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent4"/>
+                  <a:schemeClr val="accent1"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -9798,90 +10340,95 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet5!$J$128:$J$135</c:f>
+              <c:f>Sheet5!$J$1:$J$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>257</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>289</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>321</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>353</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>385</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>417</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>449</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>481</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>513</c:v>
                 </c:pt>
               </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet5!$L$127:$L$135</c:f>
+              <c:f>Sheet5!$L$1:$L$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.178259</c:v>
+                  <c:v>0.25082100000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.252695</c:v>
+                  <c:v>0.27498499999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.48150599999999999</c:v>
+                  <c:v>0.344335</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.492419</c:v>
+                  <c:v>0.45908300000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.84097500000000003</c:v>
+                  <c:v>0.70434099999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.90437500000000004</c:v>
+                  <c:v>0.95973799999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.14113</c:v>
+                  <c:v>1.05684</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.24461</c:v>
+                  <c:v>2.3274900000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.79938</c:v>
+                  <c:v>1.4976</c:v>
                 </c:pt>
               </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-C73E-4C13-8017-124647822CD5}"/>
+              <c16:uniqueId val="{00000000-C73E-4C13-8017-124647822CD5}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
+          <c:idx val="2"/>
+          <c:order val="2"/>
           <c:tx>
-            <c:v>61</c:v>
+            <c:v>75</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent6"/>
+                <a:schemeClr val="accent3"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -9892,11 +10439,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent6"/>
+                <a:schemeClr val="accent3"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent6"/>
+                  <a:schemeClr val="accent3"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -9904,7 +10451,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet5!$J$109:$J$117</c:f>
+              <c:f>Sheet5!$J$172:$J$180</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -9936,48 +10483,50 @@
                   <c:v>513</c:v>
                 </c:pt>
               </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet5!$L$109:$L$117</c:f>
+              <c:f>Sheet5!$L$172:$L$180</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.161103</c:v>
+                  <c:v>0.158579</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.29779</c:v>
+                  <c:v>0.233039</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.36225099999999999</c:v>
+                  <c:v>0.411277</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.44736999999999999</c:v>
+                  <c:v>0.49597999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.66095499999999996</c:v>
+                  <c:v>0.992309</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.98905900000000002</c:v>
+                  <c:v>1.0433600000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.24919</c:v>
+                  <c:v>1.0825</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.3903399999999999</c:v>
+                  <c:v>1.48071</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.8211599999999999</c:v>
+                  <c:v>1.7518899999999999</c:v>
                 </c:pt>
               </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-C73E-4C13-8017-124647822CD5}"/>
+              <c16:uniqueId val="{00000003-C73E-4C13-8017-124647822CD5}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -10110,129 +10659,6 @@
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredScatterSeries>
               <c15:ser>
-                <c:idx val="0"/>
-                <c:order val="0"/>
-                <c:tx>
-                  <c:v>37</c:v>
-                </c:tx>
-                <c:spPr>
-                  <a:ln w="19050" cap="rnd">
-                    <a:solidFill>
-                      <a:schemeClr val="accent1"/>
-                    </a:solidFill>
-                    <a:round/>
-                  </a:ln>
-                  <a:effectLst/>
-                </c:spPr>
-                <c:marker>
-                  <c:symbol val="circle"/>
-                  <c:size val="5"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:schemeClr val="accent1"/>
-                    </a:solidFill>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="accent1"/>
-                      </a:solidFill>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c:marker>
-                <c:xVal>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Sheet5!$J$1:$J$9</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="9"/>
-                      <c:pt idx="0">
-                        <c:v>257</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>289</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>321</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>353</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>385</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>417</c:v>
-                      </c:pt>
-                      <c:pt idx="6">
-                        <c:v>449</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>481</c:v>
-                      </c:pt>
-                      <c:pt idx="8">
-                        <c:v>513</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:xVal>
-                <c:yVal>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Sheet5!$L$1:$L$9</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="9"/>
-                      <c:pt idx="0">
-                        <c:v>0.25082100000000002</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>0.27498499999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>0.344335</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>0.45908300000000002</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>0.70434099999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>0.95973799999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="6">
-                        <c:v>1.05684</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>2.3274900000000001</c:v>
-                      </c:pt>
-                      <c:pt idx="8">
-                        <c:v>1.4976</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:yVal>
-                <c:smooth val="0"/>
-                <c:extLst>
-                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000000-C73E-4C13-8017-124647822CD5}"/>
-                  </c:ext>
-                </c:extLst>
-              </c15:ser>
-            </c15:filteredScatterSeries>
-            <c15:filteredScatterSeries>
-              <c15:ser>
                 <c:idx val="1"/>
                 <c:order val="1"/>
                 <c:tx>
@@ -10265,7 +10691,7 @@
                 <c:xVal>
                   <c:numRef>
                     <c:extLst>
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet5!$J$91:$J$99</c15:sqref>
                         </c15:formulaRef>
@@ -10307,7 +10733,7 @@
                 <c:yVal>
                   <c:numRef>
                     <c:extLst>
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet5!$M$91:$M$99</c15:sqref>
                         </c15:formulaRef>
@@ -10356,15 +10782,15 @@
             </c15:filteredScatterSeries>
             <c15:filteredScatterSeries>
               <c15:ser>
-                <c:idx val="2"/>
-                <c:order val="2"/>
+                <c:idx val="3"/>
+                <c:order val="3"/>
                 <c:tx>
-                  <c:v>75</c:v>
+                  <c:v>65</c:v>
                 </c:tx>
                 <c:spPr>
                   <a:ln w="19050" cap="rnd">
                     <a:solidFill>
-                      <a:schemeClr val="accent3"/>
+                      <a:schemeClr val="accent4"/>
                     </a:solidFill>
                     <a:round/>
                   </a:ln>
@@ -10375,11 +10801,11 @@
                   <c:size val="5"/>
                   <c:spPr>
                     <a:solidFill>
-                      <a:schemeClr val="accent3"/>
+                      <a:schemeClr val="accent4"/>
                     </a:solidFill>
                     <a:ln w="9525">
                       <a:solidFill>
-                        <a:schemeClr val="accent3"/>
+                        <a:schemeClr val="accent4"/>
                       </a:solidFill>
                     </a:ln>
                     <a:effectLst/>
@@ -10387,10 +10813,49 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet5!$J$172:$J$180</c15:sqref>
+                          <c15:sqref>Sheet5!$J$128:$J$135</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="8"/>
+                      <c:pt idx="0">
+                        <c:v>289</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>321</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>353</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>385</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>417</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>449</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>481</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>513</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet5!$L$127:$L$135</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -10398,81 +10863,39 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="9"/>
                       <c:pt idx="0">
-                        <c:v>257</c:v>
+                        <c:v>0.178259</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>289</c:v>
+                        <c:v>0.252695</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>321</c:v>
+                        <c:v>0.48150599999999999</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>353</c:v>
+                        <c:v>0.492419</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>385</c:v>
+                        <c:v>0.84097500000000003</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>417</c:v>
+                        <c:v>0.90437500000000004</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>449</c:v>
+                        <c:v>1.14113</c:v>
                       </c:pt>
                       <c:pt idx="7">
-                        <c:v>481</c:v>
+                        <c:v>1.24461</c:v>
                       </c:pt>
                       <c:pt idx="8">
-                        <c:v>513</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:xVal>
-                <c:yVal>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Sheet5!$L$172:$L$180</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="9"/>
-                      <c:pt idx="0">
-                        <c:v>0.158579</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>0.233039</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>0.411277</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>0.49597999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>0.992309</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>1.0433600000000001</c:v>
-                      </c:pt>
-                      <c:pt idx="6">
-                        <c:v>1.0825</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>1.48071</c:v>
-                      </c:pt>
-                      <c:pt idx="8">
-                        <c:v>1.7518899999999999</c:v>
+                        <c:v>1.79938</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000003-C73E-4C13-8017-124647822CD5}"/>
+                    <c16:uniqueId val="{00000004-C73E-4C13-8017-124647822CD5}"/>
                   </c:ext>
                 </c:extLst>
               </c15:ser>
@@ -10510,7 +10933,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet5!$J$28:$J$36</c15:sqref>
@@ -10552,7 +10975,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet5!$L$28:$L$36</c15:sqref>
@@ -10593,9 +11016,132 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000005-C73E-4C13-8017-124647822CD5}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="5"/>
+                <c:order val="5"/>
+                <c:tx>
+                  <c:v>61</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="19050" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent6"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent6"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent6"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet5!$J$109:$J$117</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="9"/>
+                      <c:pt idx="0">
+                        <c:v>257</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>289</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>321</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>353</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>385</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>417</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>449</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>481</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>513</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet5!$L$109:$L$117</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="9"/>
+                      <c:pt idx="0">
+                        <c:v>0.161103</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.29779</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0.36225099999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0.44736999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0.66095499999999996</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0.98905900000000002</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>1.24919</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>1.3903399999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>1.8211599999999999</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="0"/>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000006-C73E-4C13-8017-124647822CD5}"/>
                   </c:ext>
                 </c:extLst>
               </c15:ser>
@@ -10639,7 +11185,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet5!$J$136:$J$144</c15:sqref>
@@ -10681,7 +11227,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet5!$L$136:$L$144</c15:sqref>
@@ -10722,7 +11268,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000008-C73E-4C13-8017-124647822CD5}"/>
                   </c:ext>
@@ -10768,7 +11314,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet5!$J$145:$J$153</c15:sqref>
@@ -10810,7 +11356,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet5!$L$145:$L$153</c15:sqref>
@@ -10851,7 +11397,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000009-C73E-4C13-8017-124647822CD5}"/>
                   </c:ext>
@@ -10882,6 +11428,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Matrix Dimension</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -10944,6 +11545,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>AVg. Runtime (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -10993,6 +11649,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -18505,16 +19192,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>204788</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>413147</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>125017</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>438151</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>69057</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>646510</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>148829</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -18582,16 +19269,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>59531</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>140494</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>378617</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>142876</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>97631</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>169069</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>252412</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>23813</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -22474,15 +23161,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EB1B212-F208-4AAA-AB8C-B2C0436ACA7C}">
-  <dimension ref="A1:F225"/>
+  <dimension ref="A1:V225"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="O29" sqref="O29"/>
+    <sheetView topLeftCell="A205" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D225" sqref="D217:D225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A1">
         <v>256</v>
       </c>
@@ -22496,7 +23183,7 @@
         <v>0.15375900000000001</v>
       </c>
       <c r="E1">
-        <f xml:space="preserve"> (C1-D1)/C1</f>
+        <f t="shared" ref="E1:E32" si="0" xml:space="preserve"> (C1-D1)/C1</f>
         <v>0.10878297309986266</v>
       </c>
       <c r="F1">
@@ -22504,7 +23191,7 @@
         <v>1.5472719712042395</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>288</v>
       </c>
@@ -22518,11 +23205,11 @@
         <v>0.20020499999999999</v>
       </c>
       <c r="E2">
-        <f xml:space="preserve"> (C2-D2)/C2</f>
+        <f t="shared" si="0"/>
         <v>0.15476100007599361</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>320</v>
       </c>
@@ -22536,11 +23223,11 @@
         <v>0.26784400000000003</v>
       </c>
       <c r="E3">
-        <f xml:space="preserve"> (C3-D3)/C3</f>
+        <f t="shared" si="0"/>
         <v>0.15161919724305686</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>352</v>
       </c>
@@ -22554,11 +23241,23 @@
         <v>0.41627199999999998</v>
       </c>
       <c r="E4">
-        <f xml:space="preserve"> (C4-D4)/C4</f>
+        <f t="shared" si="0"/>
         <v>-3.0343083019605716E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="S4">
+        <v>256</v>
+      </c>
+      <c r="T4">
+        <v>16</v>
+      </c>
+      <c r="U4">
+        <v>0.16015499999999999</v>
+      </c>
+      <c r="V4">
+        <v>0.16816500000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>384</v>
       </c>
@@ -22572,11 +23271,23 @@
         <v>0.51048099999999996</v>
       </c>
       <c r="E5">
-        <f xml:space="preserve"> (C5-D5)/C5</f>
+        <f t="shared" si="0"/>
         <v>0.17310389959601261</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="S5">
+        <v>288</v>
+      </c>
+      <c r="T5">
+        <v>16</v>
+      </c>
+      <c r="U5">
+        <v>0.25387999999999999</v>
+      </c>
+      <c r="V5">
+        <v>0.26289899999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>416</v>
       </c>
@@ -22590,11 +23301,23 @@
         <v>0.59179000000000004</v>
       </c>
       <c r="E6">
-        <f xml:space="preserve"> (C6-D6)/C6</f>
+        <f t="shared" si="0"/>
         <v>0.23229500710898007</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="S6">
+        <v>320</v>
+      </c>
+      <c r="T6">
+        <v>16</v>
+      </c>
+      <c r="U6">
+        <v>0.31817800000000002</v>
+      </c>
+      <c r="V6">
+        <v>0.33520299999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>448</v>
       </c>
@@ -22608,11 +23331,23 @@
         <v>0.74926599999999999</v>
       </c>
       <c r="E7">
-        <f xml:space="preserve"> (C7-D7)/C7</f>
+        <f t="shared" si="0"/>
         <v>0.20506835682624022</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="S7">
+        <v>352</v>
+      </c>
+      <c r="T7">
+        <v>16</v>
+      </c>
+      <c r="U7">
+        <v>0.438527</v>
+      </c>
+      <c r="V7">
+        <v>0.426126</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>480</v>
       </c>
@@ -22626,11 +23361,23 @@
         <v>0.94081400000000004</v>
       </c>
       <c r="E8">
-        <f xml:space="preserve"> (C8-D8)/C8</f>
+        <f t="shared" si="0"/>
         <v>0.17476799466694737</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="S8">
+        <v>384</v>
+      </c>
+      <c r="T8">
+        <v>16</v>
+      </c>
+      <c r="U8">
+        <v>0.82508999999999999</v>
+      </c>
+      <c r="V8">
+        <v>0.56040599999999996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>512</v>
       </c>
@@ -22644,11 +23391,23 @@
         <v>1.02129</v>
       </c>
       <c r="E9">
-        <f xml:space="preserve"> (C9-D9)/C9</f>
+        <f t="shared" si="0"/>
         <v>0.37721662560675168</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="S9">
+        <v>416</v>
+      </c>
+      <c r="T9">
+        <v>16</v>
+      </c>
+      <c r="U9">
+        <v>0.80368600000000001</v>
+      </c>
+      <c r="V9">
+        <v>0.597109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>256</v>
       </c>
@@ -22662,15 +23421,27 @@
         <v>0.15443899999999999</v>
       </c>
       <c r="E10">
-        <f xml:space="preserve"> (C10-D10)/C10</f>
+        <f t="shared" si="0"/>
         <v>4.9161737606475018E-3</v>
       </c>
       <c r="F10">
         <f>SUM(E10:E18)</f>
         <v>1.7327056019441196</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="S10">
+        <v>448</v>
+      </c>
+      <c r="T10">
+        <v>16</v>
+      </c>
+      <c r="U10">
+        <v>0.98529800000000001</v>
+      </c>
+      <c r="V10">
+        <v>0.78029599999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>288</v>
       </c>
@@ -22684,11 +23455,23 @@
         <v>0.19211400000000001</v>
       </c>
       <c r="E11">
-        <f xml:space="preserve"> (C11-D11)/C11</f>
+        <f t="shared" si="0"/>
         <v>0.20898097328189269</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="S11">
+        <v>480</v>
+      </c>
+      <c r="T11">
+        <v>16</v>
+      </c>
+      <c r="U11">
+        <v>1.14713</v>
+      </c>
+      <c r="V11">
+        <v>0.89319999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>320</v>
       </c>
@@ -22702,11 +23485,23 @@
         <v>0.25865899999999997</v>
       </c>
       <c r="E12">
-        <f xml:space="preserve"> (C12-D12)/C12</f>
+        <f t="shared" si="0"/>
         <v>0.20573667547956609</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="S12">
+        <v>512</v>
+      </c>
+      <c r="T12">
+        <v>16</v>
+      </c>
+      <c r="U12">
+        <v>1.6994899999999999</v>
+      </c>
+      <c r="V12">
+        <v>1.06864</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>352</v>
       </c>
@@ -22720,11 +23515,23 @@
         <v>0.34215899999999999</v>
       </c>
       <c r="E13">
-        <f xml:space="preserve"> (C13-D13)/C13</f>
+        <f t="shared" si="0"/>
         <v>0.1556591435156624</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="S13">
+        <v>256</v>
+      </c>
+      <c r="T13">
+        <v>18</v>
+      </c>
+      <c r="U13">
+        <v>0.16794000000000001</v>
+      </c>
+      <c r="V13">
+        <v>0.15168599999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>384</v>
       </c>
@@ -22738,11 +23545,23 @@
         <v>0.49762600000000001</v>
       </c>
       <c r="E14">
-        <f xml:space="preserve"> (C14-D14)/C14</f>
+        <f t="shared" si="0"/>
         <v>0.19070333248222837</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="S14">
+        <v>288</v>
+      </c>
+      <c r="T14">
+        <v>18</v>
+      </c>
+      <c r="U14">
+        <v>0.242866</v>
+      </c>
+      <c r="V14">
+        <v>0.19311</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>416</v>
       </c>
@@ -22756,11 +23575,23 @@
         <v>0.56649300000000002</v>
       </c>
       <c r="E15">
-        <f xml:space="preserve"> (C15-D15)/C15</f>
+        <f t="shared" si="0"/>
         <v>0.18624982223684222</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="S15">
+        <v>320</v>
+      </c>
+      <c r="T15">
+        <v>18</v>
+      </c>
+      <c r="U15">
+        <v>0.33721600000000002</v>
+      </c>
+      <c r="V15">
+        <v>0.35042299999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>448</v>
       </c>
@@ -22774,11 +23605,23 @@
         <v>0.74224999999999997</v>
       </c>
       <c r="E16">
-        <f xml:space="preserve"> (C16-D16)/C16</f>
+        <f t="shared" si="0"/>
         <v>0.18052967205730391</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="S16">
+        <v>352</v>
+      </c>
+      <c r="T16">
+        <v>18</v>
+      </c>
+      <c r="U16">
+        <v>0.53477200000000003</v>
+      </c>
+      <c r="V16">
+        <v>0.49469299999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>480</v>
       </c>
@@ -22792,11 +23635,23 @@
         <v>0.85373200000000005</v>
       </c>
       <c r="E17">
-        <f xml:space="preserve"> (C17-D17)/C17</f>
+        <f t="shared" si="0"/>
         <v>0.23183400966357448</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="S17">
+        <v>384</v>
+      </c>
+      <c r="T17">
+        <v>18</v>
+      </c>
+      <c r="U17">
+        <v>0.63004800000000005</v>
+      </c>
+      <c r="V17">
+        <v>0.54079600000000005</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>512</v>
       </c>
@@ -22810,11 +23665,23 @@
         <v>1.01844</v>
       </c>
       <c r="E18">
-        <f xml:space="preserve"> (C18-D18)/C18</f>
+        <f t="shared" si="0"/>
         <v>0.36809579946640192</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="S18">
+        <v>416</v>
+      </c>
+      <c r="T18">
+        <v>18</v>
+      </c>
+      <c r="U18">
+        <v>0.74935799999999997</v>
+      </c>
+      <c r="V18">
+        <v>0.65441899999999997</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>256</v>
       </c>
@@ -22828,15 +23695,27 @@
         <v>0.155746</v>
       </c>
       <c r="E19">
-        <f xml:space="preserve"> (C19-D19)/C19</f>
+        <f t="shared" si="0"/>
         <v>5.8663539878635457E-2</v>
       </c>
       <c r="F19">
         <f>SUM(E19:E27)</f>
         <v>1.8733216681375964</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="S19">
+        <v>448</v>
+      </c>
+      <c r="T19">
+        <v>18</v>
+      </c>
+      <c r="U19">
+        <v>0.978931</v>
+      </c>
+      <c r="V19">
+        <v>0.76356800000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>288</v>
       </c>
@@ -22850,11 +23729,23 @@
         <v>0.197189</v>
       </c>
       <c r="E20">
-        <f xml:space="preserve"> (C20-D20)/C20</f>
+        <f t="shared" si="0"/>
         <v>0.14519121561283496</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="S20">
+        <v>480</v>
+      </c>
+      <c r="T20">
+        <v>18</v>
+      </c>
+      <c r="U20">
+        <v>1.1908700000000001</v>
+      </c>
+      <c r="V20">
+        <v>0.98223000000000005</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>320</v>
       </c>
@@ -22868,11 +23759,23 @@
         <v>0.25585000000000002</v>
       </c>
       <c r="E21">
-        <f xml:space="preserve"> (C21-D21)/C21</f>
+        <f t="shared" si="0"/>
         <v>0.22191709166993578</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="S21">
+        <v>512</v>
+      </c>
+      <c r="T21">
+        <v>18</v>
+      </c>
+      <c r="U21">
+        <v>1.6765600000000001</v>
+      </c>
+      <c r="V21">
+        <v>1.0669</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>352</v>
       </c>
@@ -22886,11 +23789,11 @@
         <v>0.334673</v>
       </c>
       <c r="E22">
-        <f xml:space="preserve"> (C22-D22)/C22</f>
+        <f t="shared" si="0"/>
         <v>0.18191662551882945</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>384</v>
       </c>
@@ -22904,11 +23807,11 @@
         <v>0.431398</v>
       </c>
       <c r="E23">
-        <f xml:space="preserve"> (C23-D23)/C23</f>
+        <f t="shared" si="0"/>
         <v>0.27512946577096398</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>416</v>
       </c>
@@ -22922,11 +23825,11 @@
         <v>0.56309799999999999</v>
       </c>
       <c r="E24">
-        <f xml:space="preserve"> (C24-D24)/C24</f>
+        <f t="shared" si="0"/>
         <v>0.18790579616089065</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>448</v>
       </c>
@@ -22940,11 +23843,11 @@
         <v>0.69981199999999999</v>
       </c>
       <c r="E25">
-        <f xml:space="preserve"> (C25-D25)/C25</f>
+        <f t="shared" si="0"/>
         <v>0.23281706322408638</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>480</v>
       </c>
@@ -22958,11 +23861,11 @@
         <v>0.89319300000000001</v>
       </c>
       <c r="E26">
-        <f xml:space="preserve"> (C26-D26)/C26</f>
+        <f t="shared" si="0"/>
         <v>0.20036436884512085</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A27">
         <v>512</v>
       </c>
@@ -22976,11 +23879,11 @@
         <v>1.0305500000000001</v>
       </c>
       <c r="E27">
-        <f xml:space="preserve"> (C27-D27)/C27</f>
+        <f t="shared" si="0"/>
         <v>0.36941650145629873</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A28">
         <v>256</v>
       </c>
@@ -22994,7 +23897,7 @@
         <v>0.148336</v>
       </c>
       <c r="E28">
-        <f xml:space="preserve"> (C28-D28)/C28</f>
+        <f t="shared" si="0"/>
         <v>0.13799736173823107</v>
       </c>
       <c r="F28">
@@ -23002,7 +23905,7 @@
         <v>2.2655390511383144</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>288</v>
       </c>
@@ -23016,11 +23919,11 @@
         <v>0.19017300000000001</v>
       </c>
       <c r="E29">
-        <f xml:space="preserve"> (C29-D29)/C29</f>
+        <f t="shared" si="0"/>
         <v>0.24406735195210955</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A30">
         <v>320</v>
       </c>
@@ -23034,11 +23937,11 @@
         <v>0.26335599999999998</v>
       </c>
       <c r="E30">
-        <f xml:space="preserve"> (C30-D30)/C30</f>
+        <f t="shared" si="0"/>
         <v>0.17194063639793741</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A31">
         <v>352</v>
       </c>
@@ -23052,11 +23955,11 @@
         <v>0.31091800000000003</v>
       </c>
       <c r="E31">
-        <f xml:space="preserve"> (C31-D31)/C31</f>
+        <f t="shared" si="0"/>
         <v>0.2699793145387564</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>384</v>
       </c>
@@ -23070,7 +23973,7 @@
         <v>0.41486099999999998</v>
       </c>
       <c r="E32">
-        <f xml:space="preserve"> (C32-D32)/C32</f>
+        <f t="shared" si="0"/>
         <v>0.31552384095033825</v>
       </c>
     </row>
@@ -23088,7 +23991,7 @@
         <v>0.51500000000000001</v>
       </c>
       <c r="E33">
-        <f xml:space="preserve"> (C33-D33)/C33</f>
+        <f t="shared" ref="E33:E64" si="1" xml:space="preserve"> (C33-D33)/C33</f>
         <v>0.26877024193056009</v>
       </c>
     </row>
@@ -23106,7 +24009,7 @@
         <v>0.70112300000000005</v>
       </c>
       <c r="E34">
-        <f xml:space="preserve"> (C34-D34)/C34</f>
+        <f t="shared" si="1"/>
         <v>0.24834391292182106</v>
       </c>
     </row>
@@ -23124,7 +24027,7 @@
         <v>0.85660700000000001</v>
       </c>
       <c r="E35">
-        <f xml:space="preserve"> (C35-D35)/C35</f>
+        <f t="shared" si="1"/>
         <v>0.2330838443976902</v>
       </c>
     </row>
@@ -23142,7 +24045,7 @@
         <v>1.0111699999999999</v>
       </c>
       <c r="E36">
-        <f xml:space="preserve"> (C36-D36)/C36</f>
+        <f t="shared" si="1"/>
         <v>0.37583254631087087</v>
       </c>
     </row>
@@ -23160,7 +24063,7 @@
         <v>0.14141599999999999</v>
       </c>
       <c r="E37">
-        <f xml:space="preserve"> (C37-D37)/C37</f>
+        <f t="shared" si="1"/>
         <v>0.18149721601629887</v>
       </c>
       <c r="F37">
@@ -23182,7 +24085,7 @@
         <v>0.20425099999999999</v>
       </c>
       <c r="E38">
-        <f xml:space="preserve"> (C38-D38)/C38</f>
+        <f t="shared" si="1"/>
         <v>0.10163266742318289</v>
       </c>
     </row>
@@ -23200,7 +24103,7 @@
         <v>0.26256800000000002</v>
       </c>
       <c r="E39">
-        <f xml:space="preserve"> (C39-D39)/C39</f>
+        <f t="shared" si="1"/>
         <v>0.19385956832765336</v>
       </c>
     </row>
@@ -23218,7 +24121,7 @@
         <v>0.30882199999999999</v>
       </c>
       <c r="E40">
-        <f xml:space="preserve"> (C40-D40)/C40</f>
+        <f t="shared" si="1"/>
         <v>0.30446748707230503</v>
       </c>
     </row>
@@ -23236,7 +24139,7 @@
         <v>0.415684</v>
       </c>
       <c r="E41">
-        <f xml:space="preserve"> (C41-D41)/C41</f>
+        <f t="shared" si="1"/>
         <v>0.31912231045417622</v>
       </c>
     </row>
@@ -23254,7 +24157,7 @@
         <v>0.50359200000000004</v>
       </c>
       <c r="E42">
-        <f xml:space="preserve"> (C42-D42)/C42</f>
+        <f t="shared" si="1"/>
         <v>0.29630442164275561</v>
       </c>
     </row>
@@ -23272,7 +24175,7 @@
         <v>0.60124599999999995</v>
       </c>
       <c r="E43">
-        <f xml:space="preserve"> (C43-D43)/C43</f>
+        <f t="shared" si="1"/>
         <v>0.37083084367305386</v>
       </c>
     </row>
@@ -23290,7 +24193,7 @@
         <v>0.88881399999999999</v>
       </c>
       <c r="E44">
-        <f xml:space="preserve"> (C44-D44)/C44</f>
+        <f t="shared" si="1"/>
         <v>0.20704618651250342</v>
       </c>
     </row>
@@ -23308,7 +24211,7 @@
         <v>1.0144200000000001</v>
       </c>
       <c r="E45">
-        <f xml:space="preserve"> (C45-D45)/C45</f>
+        <f t="shared" si="1"/>
         <v>0.38752739589559665</v>
       </c>
     </row>
@@ -23326,7 +24229,7 @@
         <v>0.14534900000000001</v>
       </c>
       <c r="E46">
-        <f xml:space="preserve"> (C46-D46)/C46</f>
+        <f t="shared" si="1"/>
         <v>0.1721166278400838</v>
       </c>
       <c r="F46">
@@ -23348,7 +24251,7 @@
         <v>0.205843</v>
       </c>
       <c r="E47">
-        <f xml:space="preserve"> (C47-D47)/C47</f>
+        <f t="shared" si="1"/>
         <v>0.13664064826504374</v>
       </c>
     </row>
@@ -23366,7 +24269,7 @@
         <v>0.249111</v>
       </c>
       <c r="E48">
-        <f xml:space="preserve"> (C48-D48)/C48</f>
+        <f t="shared" si="1"/>
         <v>0.19169668061909867</v>
       </c>
     </row>
@@ -23384,7 +24287,7 @@
         <v>0.30514599999999997</v>
       </c>
       <c r="E49">
-        <f xml:space="preserve"> (C49-D49)/C49</f>
+        <f t="shared" si="1"/>
         <v>0.29943131857409505</v>
       </c>
     </row>
@@ -23402,7 +24305,7 @@
         <v>0.39258599999999999</v>
       </c>
       <c r="E50">
-        <f xml:space="preserve"> (C50-D50)/C50</f>
+        <f t="shared" si="1"/>
         <v>0.35859192345960994</v>
       </c>
     </row>
@@ -23420,7 +24323,7 @@
         <v>0.50529000000000002</v>
       </c>
       <c r="E51">
-        <f xml:space="preserve"> (C51-D51)/C51</f>
+        <f t="shared" si="1"/>
         <v>0.29758884571809863</v>
       </c>
     </row>
@@ -23438,7 +24341,7 @@
         <v>0.58956600000000003</v>
       </c>
       <c r="E52">
-        <f xml:space="preserve"> (C52-D52)/C52</f>
+        <f t="shared" si="1"/>
         <v>0.3666008807505825</v>
       </c>
     </row>
@@ -23456,7 +24359,7 @@
         <v>0.75526700000000002</v>
       </c>
       <c r="E53">
-        <f xml:space="preserve"> (C53-D53)/C53</f>
+        <f t="shared" si="1"/>
         <v>0.3219737503590922</v>
       </c>
     </row>
@@ -23474,7 +24377,7 @@
         <v>0.99872399999999995</v>
       </c>
       <c r="E54">
-        <f xml:space="preserve"> (C54-D54)/C54</f>
+        <f t="shared" si="1"/>
         <v>0.36346868407467131</v>
       </c>
     </row>
@@ -23492,7 +24395,7 @@
         <v>0.12649099999999999</v>
       </c>
       <c r="E55">
-        <f xml:space="preserve"> (C55-D55)/C55</f>
+        <f t="shared" si="1"/>
         <v>0.22791308063236287</v>
       </c>
       <c r="F55">
@@ -23514,7 +24417,7 @@
         <v>0.190105</v>
       </c>
       <c r="E56">
-        <f xml:space="preserve"> (C56-D56)/C56</f>
+        <f t="shared" si="1"/>
         <v>0.21997964861027908</v>
       </c>
     </row>
@@ -23532,7 +24435,7 @@
         <v>0.238395</v>
       </c>
       <c r="E57">
-        <f xml:space="preserve"> (C57-D57)/C57</f>
+        <f t="shared" si="1"/>
         <v>0.26161722846673957</v>
       </c>
     </row>
@@ -23550,7 +24453,7 @@
         <v>0.33472600000000002</v>
       </c>
       <c r="E58">
-        <f xml:space="preserve"> (C58-D58)/C58</f>
+        <f t="shared" si="1"/>
         <v>0.20621038178148873</v>
       </c>
     </row>
@@ -23568,7 +24471,7 @@
         <v>0.40362500000000001</v>
       </c>
       <c r="E59">
-        <f xml:space="preserve"> (C59-D59)/C59</f>
+        <f t="shared" si="1"/>
         <v>0.32300856753728585</v>
       </c>
     </row>
@@ -23586,7 +24489,7 @@
         <v>0.51046000000000002</v>
       </c>
       <c r="E60">
-        <f xml:space="preserve"> (C60-D60)/C60</f>
+        <f t="shared" si="1"/>
         <v>0.26780499279939868</v>
       </c>
     </row>
@@ -23604,7 +24507,7 @@
         <v>0.63260099999999997</v>
       </c>
       <c r="E61">
-        <f xml:space="preserve"> (C61-D61)/C61</f>
+        <f t="shared" si="1"/>
         <v>0.34626505675476815</v>
       </c>
     </row>
@@ -23622,7 +24525,7 @@
         <v>0.742089</v>
       </c>
       <c r="E62">
-        <f xml:space="preserve"> (C62-D62)/C62</f>
+        <f t="shared" si="1"/>
         <v>0.33250371036653925</v>
       </c>
     </row>
@@ -23640,7 +24543,7 @@
         <v>0.87779499999999999</v>
       </c>
       <c r="E63">
-        <f xml:space="preserve"> (C63-D63)/C63</f>
+        <f t="shared" si="1"/>
         <v>0.43108934890533657</v>
       </c>
     </row>
@@ -23658,7 +24561,7 @@
         <v>0.122728</v>
       </c>
       <c r="E64">
-        <f xml:space="preserve"> (C64-D64)/C64</f>
+        <f t="shared" si="1"/>
         <v>0.2716612068556235</v>
       </c>
       <c r="F64">
@@ -23680,7 +24583,7 @@
         <v>0.204568</v>
       </c>
       <c r="E65">
-        <f xml:space="preserve"> (C65-D65)/C65</f>
+        <f t="shared" ref="E65:E96" si="2" xml:space="preserve"> (C65-D65)/C65</f>
         <v>9.8163863601296128E-2</v>
       </c>
     </row>
@@ -23698,7 +24601,7 @@
         <v>0.25834000000000001</v>
       </c>
       <c r="E66">
-        <f xml:space="preserve"> (C66-D66)/C66</f>
+        <f t="shared" si="2"/>
         <v>0.16995463249752599</v>
       </c>
     </row>
@@ -23716,7 +24619,7 @@
         <v>0.33545599999999998</v>
       </c>
       <c r="E67">
-        <f xml:space="preserve"> (C67-D67)/C67</f>
+        <f t="shared" si="2"/>
         <v>0.17089880920015235</v>
       </c>
     </row>
@@ -23734,7 +24637,7 @@
         <v>0.42746200000000001</v>
       </c>
       <c r="E68">
-        <f xml:space="preserve"> (C68-D68)/C68</f>
+        <f t="shared" si="2"/>
         <v>0.32835565276278555</v>
       </c>
     </row>
@@ -23752,7 +24655,7 @@
         <v>0.50649299999999997</v>
       </c>
       <c r="E69">
-        <f xml:space="preserve"> (C69-D69)/C69</f>
+        <f t="shared" si="2"/>
         <v>0.26386111272600432</v>
       </c>
     </row>
@@ -23770,7 +24673,7 @@
         <v>0.62167300000000003</v>
       </c>
       <c r="E70">
-        <f xml:space="preserve"> (C70-D70)/C70</f>
+        <f t="shared" si="2"/>
         <v>0.35821340821340814</v>
       </c>
     </row>
@@ -23788,7 +24691,7 @@
         <v>0.76271500000000003</v>
       </c>
       <c r="E71">
-        <f xml:space="preserve"> (C71-D71)/C71</f>
+        <f t="shared" si="2"/>
         <v>0.31601201685947444</v>
       </c>
     </row>
@@ -23806,7 +24709,7 @@
         <v>0.88406099999999999</v>
       </c>
       <c r="E72">
-        <f xml:space="preserve"> (C72-D72)/C72</f>
+        <f t="shared" si="2"/>
         <v>0.42343346463882298</v>
       </c>
     </row>
@@ -23824,7 +24727,7 @@
         <v>0.13633899999999999</v>
       </c>
       <c r="E73">
-        <f xml:space="preserve"> (C73-D73)/C73</f>
+        <f t="shared" si="2"/>
         <v>0.17561161432320332</v>
       </c>
       <c r="F73">
@@ -23846,7 +24749,7 @@
         <v>0.17882899999999999</v>
       </c>
       <c r="E74">
-        <f xml:space="preserve"> (C74-D74)/C74</f>
+        <f t="shared" si="2"/>
         <v>0.27985035558669791</v>
       </c>
     </row>
@@ -23864,7 +24767,7 @@
         <v>0.247697</v>
       </c>
       <c r="E75">
-        <f xml:space="preserve"> (C75-D75)/C75</f>
+        <f t="shared" si="2"/>
         <v>0.23238286491696183</v>
       </c>
     </row>
@@ -23882,7 +24785,7 @@
         <v>0.32827400000000001</v>
       </c>
       <c r="E76">
-        <f xml:space="preserve"> (C76-D76)/C76</f>
+        <f t="shared" si="2"/>
         <v>0.200495863340453</v>
       </c>
     </row>
@@ -23900,7 +24803,7 @@
         <v>0.406555</v>
       </c>
       <c r="E77">
-        <f xml:space="preserve"> (C77-D77)/C77</f>
+        <f t="shared" si="2"/>
         <v>0.33642632717182841</v>
       </c>
     </row>
@@ -23918,7 +24821,7 @@
         <v>0.50383999999999995</v>
       </c>
       <c r="E78">
-        <f xml:space="preserve"> (C78-D78)/C78</f>
+        <f t="shared" si="2"/>
         <v>0.27844736721506813</v>
       </c>
     </row>
@@ -23936,7 +24839,7 @@
         <v>0.68417399999999995</v>
       </c>
       <c r="E79">
-        <f xml:space="preserve"> (C79-D79)/C79</f>
+        <f t="shared" si="2"/>
         <v>0.25608517615641729</v>
       </c>
     </row>
@@ -23954,7 +24857,7 @@
         <v>0.74207900000000004</v>
       </c>
       <c r="E80">
-        <f xml:space="preserve"> (C80-D80)/C80</f>
+        <f t="shared" si="2"/>
         <v>0.33590560482535808</v>
       </c>
     </row>
@@ -23972,7 +24875,7 @@
         <v>0.86065800000000003</v>
       </c>
       <c r="E81">
-        <f xml:space="preserve"> (C81-D81)/C81</f>
+        <f t="shared" si="2"/>
         <v>0.44857540091876547</v>
       </c>
     </row>
@@ -23990,7 +24893,7 @@
         <v>0.132601</v>
       </c>
       <c r="E82">
-        <f xml:space="preserve"> (C82-D82)/C82</f>
+        <f t="shared" si="2"/>
         <v>0.18333045920378407</v>
       </c>
       <c r="F82">
@@ -24012,7 +24915,7 @@
         <v>0.18223500000000001</v>
       </c>
       <c r="E83">
-        <f xml:space="preserve"> (C83-D83)/C83</f>
+        <f t="shared" si="2"/>
         <v>0.20389761870437595</v>
       </c>
     </row>
@@ -24030,7 +24933,7 @@
         <v>0.25304100000000002</v>
       </c>
       <c r="E84">
-        <f xml:space="preserve"> (C84-D84)/C84</f>
+        <f t="shared" si="2"/>
         <v>0.17175317661383763</v>
       </c>
     </row>
@@ -24048,7 +24951,7 @@
         <v>0.31466100000000002</v>
       </c>
       <c r="E85">
-        <f xml:space="preserve"> (C85-D85)/C85</f>
+        <f t="shared" si="2"/>
         <v>0.27599393480606793</v>
       </c>
     </row>
@@ -24066,7 +24969,7 @@
         <v>0.40060299999999999</v>
       </c>
       <c r="E86">
-        <f xml:space="preserve"> (C86-D86)/C86</f>
+        <f t="shared" si="2"/>
         <v>0.39973418282946943</v>
       </c>
     </row>
@@ -24084,7 +24987,7 @@
         <v>0.49884499999999998</v>
       </c>
       <c r="E87">
-        <f xml:space="preserve"> (C87-D87)/C87</f>
+        <f t="shared" si="2"/>
         <v>0.3537858669602954</v>
       </c>
     </row>
@@ -24102,7 +25005,7 @@
         <v>0.68686999999999998</v>
       </c>
       <c r="E88">
-        <f xml:space="preserve"> (C88-D88)/C88</f>
+        <f t="shared" si="2"/>
         <v>0.23695863244217233</v>
       </c>
     </row>
@@ -24120,7 +25023,7 @@
         <v>0.76136899999999996</v>
       </c>
       <c r="E89">
-        <f xml:space="preserve"> (C89-D89)/C89</f>
+        <f t="shared" si="2"/>
         <v>0.33499082889335319</v>
       </c>
     </row>
@@ -24138,7 +25041,7 @@
         <v>0.97066300000000005</v>
       </c>
       <c r="E90">
-        <f xml:space="preserve"> (C90-D90)/C90</f>
+        <f t="shared" si="2"/>
         <v>0.38639033055395761</v>
       </c>
     </row>
@@ -24156,7 +25059,7 @@
         <v>0.129555</v>
       </c>
       <c r="E91">
-        <f xml:space="preserve"> (C91-D91)/C91</f>
+        <f t="shared" si="2"/>
         <v>0.23146511324403524</v>
       </c>
       <c r="F91">
@@ -24178,7 +25081,7 @@
         <v>0.17181199999999999</v>
       </c>
       <c r="E92">
-        <f xml:space="preserve"> (C92-D92)/C92</f>
+        <f t="shared" si="2"/>
         <v>0.28528106293496847</v>
       </c>
     </row>
@@ -24196,7 +25099,7 @@
         <v>0.234626</v>
       </c>
       <c r="E93">
-        <f xml:space="preserve"> (C93-D93)/C93</f>
+        <f t="shared" si="2"/>
         <v>0.27048691001803377</v>
       </c>
     </row>
@@ -24214,7 +25117,7 @@
         <v>0.31314799999999998</v>
       </c>
       <c r="E94">
-        <f xml:space="preserve"> (C94-D94)/C94</f>
+        <f t="shared" si="2"/>
         <v>0.25492929932213965</v>
       </c>
     </row>
@@ -24232,7 +25135,7 @@
         <v>0.41129300000000002</v>
       </c>
       <c r="E95">
-        <f xml:space="preserve"> (C95-D95)/C95</f>
+        <f t="shared" si="2"/>
         <v>0.31943555045909511</v>
       </c>
     </row>
@@ -24250,7 +25153,7 @@
         <v>0.50698799999999999</v>
       </c>
       <c r="E96">
-        <f xml:space="preserve"> (C96-D96)/C96</f>
+        <f t="shared" si="2"/>
         <v>0.28294297352342163</v>
       </c>
     </row>
@@ -24268,7 +25171,7 @@
         <v>0.65803699999999998</v>
       </c>
       <c r="E97">
-        <f xml:space="preserve"> (C97-D97)/C97</f>
+        <f t="shared" ref="E97:E128" si="3" xml:space="preserve"> (C97-D97)/C97</f>
         <v>0.25342266041150213</v>
       </c>
     </row>
@@ -24286,7 +25189,7 @@
         <v>0.74580100000000005</v>
       </c>
       <c r="E98">
-        <f xml:space="preserve"> (C98-D98)/C98</f>
+        <f t="shared" si="3"/>
         <v>0.32964118144066729</v>
       </c>
     </row>
@@ -24304,7 +25207,7 @@
         <v>0.87202999999999997</v>
       </c>
       <c r="E99">
-        <f xml:space="preserve"> (C99-D99)/C99</f>
+        <f t="shared" si="3"/>
         <v>0.43848679974243399</v>
       </c>
     </row>
@@ -24322,7 +25225,7 @@
         <v>0.12814600000000001</v>
       </c>
       <c r="E100">
-        <f xml:space="preserve"> (C100-D100)/C100</f>
+        <f t="shared" si="3"/>
         <v>0.24597822889085014</v>
       </c>
       <c r="F100">
@@ -24344,7 +25247,7 @@
         <v>0.24682599999999999</v>
       </c>
       <c r="E101">
-        <f xml:space="preserve"> (C101-D101)/C101</f>
+        <f t="shared" si="3"/>
         <v>0.25221237597515722</v>
       </c>
     </row>
@@ -24362,7 +25265,7 @@
         <v>0.235592</v>
       </c>
       <c r="E102">
-        <f xml:space="preserve"> (C102-D102)/C102</f>
+        <f t="shared" si="3"/>
         <v>0.25876937694870672</v>
       </c>
     </row>
@@ -24380,7 +25283,7 @@
         <v>0.33012200000000003</v>
       </c>
       <c r="E103">
-        <f xml:space="preserve"> (C103-D103)/C103</f>
+        <f t="shared" si="3"/>
         <v>0.21166589852397194</v>
       </c>
     </row>
@@ -24398,7 +25301,7 @@
         <v>0.40737499999999999</v>
       </c>
       <c r="E104">
-        <f xml:space="preserve"> (C104-D104)/C104</f>
+        <f t="shared" si="3"/>
         <v>0.32544985188460085</v>
       </c>
     </row>
@@ -24416,7 +25319,7 @@
         <v>0.52664299999999997</v>
       </c>
       <c r="E105">
-        <f xml:space="preserve"> (C105-D105)/C105</f>
+        <f t="shared" si="3"/>
         <v>0.27279543552765673</v>
       </c>
     </row>
@@ -24434,7 +25337,7 @@
         <v>0.654034</v>
       </c>
       <c r="E106">
-        <f xml:space="preserve"> (C106-D106)/C106</f>
+        <f t="shared" si="3"/>
         <v>0.26109541993356988</v>
       </c>
     </row>
@@ -24452,7 +25355,7 @@
         <v>0.76277300000000003</v>
       </c>
       <c r="E107">
-        <f xml:space="preserve"> (C107-D107)/C107</f>
+        <f t="shared" si="3"/>
         <v>0.30569264798245055</v>
       </c>
     </row>
@@ -24470,7 +25373,7 @@
         <v>0.89594799999999997</v>
       </c>
       <c r="E108">
-        <f xml:space="preserve"> (C108-D108)/C108</f>
+        <f t="shared" si="3"/>
         <v>0.43225798275130062</v>
       </c>
     </row>
@@ -24488,7 +25391,7 @@
         <v>0.122033</v>
       </c>
       <c r="E109">
-        <f xml:space="preserve"> (C109-D109)/C109</f>
+        <f t="shared" si="3"/>
         <v>0.34658899246638791</v>
       </c>
       <c r="F109">
@@ -24510,7 +25413,7 @@
         <v>0.218032</v>
       </c>
       <c r="E110">
-        <f xml:space="preserve"> (C110-D110)/C110</f>
+        <f t="shared" si="3"/>
         <v>0.3612880168267118</v>
       </c>
     </row>
@@ -24528,7 +25431,7 @@
         <v>0.24024300000000001</v>
       </c>
       <c r="E111">
-        <f xml:space="preserve"> (C111-D111)/C111</f>
+        <f t="shared" si="3"/>
         <v>0.23143145064542442</v>
       </c>
     </row>
@@ -24546,7 +25449,7 @@
         <v>0.32571800000000001</v>
       </c>
       <c r="E112">
-        <f xml:space="preserve"> (C112-D112)/C112</f>
+        <f t="shared" si="3"/>
         <v>0.20006974750910525</v>
       </c>
     </row>
@@ -24564,7 +25467,7 @@
         <v>0.42416799999999999</v>
       </c>
       <c r="E113">
-        <f xml:space="preserve"> (C113-D113)/C113</f>
+        <f t="shared" si="3"/>
         <v>0.2982939083279707</v>
       </c>
     </row>
@@ -24582,7 +25485,7 @@
         <v>0.500112</v>
       </c>
       <c r="E114">
-        <f xml:space="preserve"> (C114-D114)/C114</f>
+        <f t="shared" si="3"/>
         <v>0.27561993047508693</v>
       </c>
     </row>
@@ -24600,7 +25503,7 @@
         <v>0.65186500000000003</v>
       </c>
       <c r="E115">
-        <f xml:space="preserve"> (C115-D115)/C115</f>
+        <f t="shared" si="3"/>
         <v>0.2581526223248985</v>
       </c>
     </row>
@@ -24618,7 +25521,7 @@
         <v>0.76257200000000003</v>
       </c>
       <c r="E116">
-        <f xml:space="preserve"> (C116-D116)/C116</f>
+        <f t="shared" si="3"/>
         <v>0.30784758654491978</v>
       </c>
     </row>
@@ -24636,7 +25539,7 @@
         <v>0.90410199999999996</v>
       </c>
       <c r="E117">
-        <f xml:space="preserve"> (C117-D117)/C117</f>
+        <f t="shared" si="3"/>
         <v>0.42896536914108147</v>
       </c>
     </row>
@@ -24654,7 +25557,7 @@
         <v>0.12679399999999999</v>
       </c>
       <c r="E118">
-        <f xml:space="preserve"> (C118-D118)/C118</f>
+        <f t="shared" si="3"/>
         <v>0.25788968488083541</v>
       </c>
       <c r="F118">
@@ -24676,7 +25579,7 @@
         <v>0.17943799999999999</v>
       </c>
       <c r="E119">
-        <f xml:space="preserve"> (C119-D119)/C119</f>
+        <f t="shared" si="3"/>
         <v>0.22967484910147773</v>
       </c>
     </row>
@@ -24694,7 +25597,7 @@
         <v>0.22573399999999999</v>
       </c>
       <c r="E120">
-        <f xml:space="preserve"> (C120-D120)/C120</f>
+        <f t="shared" si="3"/>
         <v>0.29680291329580605</v>
       </c>
     </row>
@@ -24712,7 +25615,7 @@
         <v>0.29196499999999997</v>
       </c>
       <c r="E121">
-        <f xml:space="preserve"> (C121-D121)/C121</f>
+        <f t="shared" si="3"/>
         <v>0.3297359715516866</v>
       </c>
     </row>
@@ -24730,7 +25633,7 @@
         <v>0.41719299999999998</v>
       </c>
       <c r="E122">
-        <f xml:space="preserve"> (C122-D122)/C122</f>
+        <f t="shared" si="3"/>
         <v>0.3172466839594465</v>
       </c>
     </row>
@@ -24748,7 +25651,7 @@
         <v>0.50188699999999997</v>
       </c>
       <c r="E123">
-        <f xml:space="preserve"> (C123-D123)/C123</f>
+        <f t="shared" si="3"/>
         <v>0.28528727382508673</v>
       </c>
     </row>
@@ -24766,7 +25669,7 @@
         <v>0.66224499999999997</v>
       </c>
       <c r="E124">
-        <f xml:space="preserve"> (C124-D124)/C124</f>
+        <f t="shared" si="3"/>
         <v>0.23985344470372713</v>
       </c>
     </row>
@@ -24784,7 +25687,7 @@
         <v>0.73905799999999999</v>
       </c>
       <c r="E125">
-        <f xml:space="preserve"> (C125-D125)/C125</f>
+        <f t="shared" si="3"/>
         <v>0.3277440716046463</v>
       </c>
     </row>
@@ -24802,7 +25705,7 @@
         <v>0.88100000000000001</v>
       </c>
       <c r="E126">
-        <f xml:space="preserve"> (C126-D126)/C126</f>
+        <f t="shared" si="3"/>
         <v>0.43991659143790768</v>
       </c>
     </row>
@@ -24820,7 +25723,7 @@
         <v>0.13094600000000001</v>
       </c>
       <c r="E127">
-        <f xml:space="preserve"> (C127-D127)/C127</f>
+        <f t="shared" si="3"/>
         <v>0.19587084413112085</v>
       </c>
       <c r="F127">
@@ -24842,7 +25745,7 @@
         <v>0.176117</v>
       </c>
       <c r="E128">
-        <f xml:space="preserve"> (C128-D128)/C128</f>
+        <f t="shared" si="3"/>
         <v>0.23509203200055598</v>
       </c>
     </row>
@@ -24860,7 +25763,7 @@
         <v>0.236017</v>
       </c>
       <c r="E129">
-        <f xml:space="preserve"> (C129-D129)/C129</f>
+        <f t="shared" ref="E129:E135" si="4" xml:space="preserve"> (C129-D129)/C129</f>
         <v>0.24299661938943734</v>
       </c>
     </row>
@@ -24878,7 +25781,7 @@
         <v>0.29710599999999998</v>
       </c>
       <c r="E130">
-        <f xml:space="preserve"> (C130-D130)/C130</f>
+        <f t="shared" si="4"/>
         <v>0.32620163196066609</v>
       </c>
     </row>
@@ -24896,7 +25799,7 @@
         <v>0.37909399999999999</v>
       </c>
       <c r="E131">
-        <f xml:space="preserve"> (C131-D131)/C131</f>
+        <f t="shared" si="4"/>
         <v>0.38943353803981068</v>
       </c>
     </row>
@@ -24914,7 +25817,7 @@
         <v>0.49939800000000001</v>
       </c>
       <c r="E132">
-        <f xml:space="preserve"> (C132-D132)/C132</f>
+        <f t="shared" si="4"/>
         <v>0.30251286320035303</v>
       </c>
     </row>
@@ -24932,7 +25835,7 @@
         <v>0.62651800000000002</v>
       </c>
       <c r="E133">
-        <f xml:space="preserve"> (C133-D133)/C133</f>
+        <f t="shared" si="4"/>
         <v>0.29587867658214828</v>
       </c>
     </row>
@@ -24950,7 +25853,7 @@
         <v>0.74869799999999997</v>
       </c>
       <c r="E134">
-        <f xml:space="preserve"> (C134-D134)/C134</f>
+        <f t="shared" si="4"/>
         <v>0.31531335448883857</v>
       </c>
     </row>
@@ -24968,7 +25871,7 @@
         <v>0.88266500000000003</v>
       </c>
       <c r="E135">
-        <f xml:space="preserve"> (C135-D135)/C135</f>
+        <f t="shared" si="4"/>
         <v>0.44197286566862232</v>
       </c>
     </row>
@@ -26233,8 +27136,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:F225">
-    <sortCondition ref="B2"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="S4:V21">
+    <sortCondition ref="T6"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -26245,8 +27148,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C49D167-98FB-46AF-A4FD-4836520472C4}">
   <dimension ref="A1:M180"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+    <sheetView tabSelected="1" topLeftCell="A160" workbookViewId="0">
+      <selection activeCell="O174" sqref="O174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>